<commit_message>
keep burning bug fixed
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25480" yWindow="1400" windowWidth="24060" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="25680" yWindow="5420" windowWidth="24060" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -137,8 +137,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="601">
+  <cellStyleXfs count="613">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -766,7 +778,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="601">
+  <cellStyles count="613">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1067,6 +1079,12 @@
     <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1367,6 +1385,12 @@
     <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2771,11 +2795,10 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="O15" t="str">
         <f t="shared" si="11"/>
         <v>false</v>
@@ -2802,7 +2825,7 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="18"/>
@@ -2818,7 +2841,7 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, true, false, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -2839,22 +2862,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
       <c r="O16" t="str">
         <f t="shared" si="11"/>
         <v>false</v>
@@ -2873,15 +2886,15 @@
       </c>
       <c r="S16" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="18"/>
@@ -2889,15 +2902,15 @@
       </c>
       <c r="W16" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, true, true, true, false, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -2917,27 +2930,13 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
       <c r="O17" t="str">
         <f t="shared" si="11"/>
         <v>false</v>
@@ -2952,35 +2951,35 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, true, true, true, true, true, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -2997,7 +2996,9 @@
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E18" s="7" t="s">
         <v>0</v>
       </c>
@@ -3008,7 +3009,9 @@
       <c r="H18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="J18" s="7" t="s">
         <v>0</v>
       </c>
@@ -3023,7 +3026,7 @@
       </c>
       <c r="O18" t="str">
         <f t="shared" si="11"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="12"/>
@@ -3043,7 +3046,7 @@
       </c>
       <c r="T18" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U18" t="str">
         <f t="shared" si="17"/>
@@ -3063,7 +3066,7 @@
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, false, true, true, false, true, true, true, true}</v>
+        <v>{true, true, false, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -3098,9 +3101,7 @@
       <c r="I19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="J19" s="1"/>
       <c r="K19" s="7" t="s">
         <v>0</v>
       </c>
@@ -3136,7 +3137,7 @@
       </c>
       <c r="U19" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="18"/>
@@ -3152,7 +3153,7 @@
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, false, true, true, true}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -3175,13 +3176,13 @@
       <c r="E20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="I20" s="7" t="s">
         <v>0</v>
       </c>
@@ -3207,7 +3208,7 @@
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="13"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="14"/>
@@ -3215,7 +3216,7 @@
       </c>
       <c r="S20" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T20" t="str">
         <f t="shared" si="16"/>
@@ -3239,7 +3240,7 @@
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, false, true, true, true, true, true}</v>
+        <v>{true, true, false, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -3259,13 +3260,13 @@
       <c r="D21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="F21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="7" t="s">
         <v>0</v>
       </c>
@@ -3290,7 +3291,7 @@
       </c>
       <c r="P21" t="str">
         <f t="shared" si="12"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="13"/>
@@ -3298,7 +3299,7 @@
       </c>
       <c r="R21" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="15"/>
@@ -3326,7 +3327,7 @@
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="10"/>
-        <v>{true, false, true, true, true, true, true, true, true, true}</v>
+        <v>{true, true, true, false, true, true, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -3384,7 +3385,7 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, false, true, true, false, true, true, true, true}, {false, false, false, true, true, true, true, true, true, true}, {false, false, false, false, true, true, true, false, true, true}, {false, false, false, false, false, false, true, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">

</xml_diff>

<commit_message>
way to test best_strategies
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="5420" windowWidth="24060" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="20460" yWindow="4300" windowWidth="24060" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="visual" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="best strategy compiler" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -137,8 +137,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="613">
+  <cellStyleXfs count="615">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -778,7 +780,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="613">
+  <cellStyles count="615">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1085,6 +1087,7 @@
     <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1391,6 +1394,7 @@
     <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3406,7 +3410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -3476,362 +3480,915 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:C94"/>
+  <dimension ref="A3:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92:C94"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="42.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="3:3">
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE("go playGames(",A3,",",B3,",",C3,",",D3,", 10, TRUE)")</f>
+        <v>go playGames(7,1,2,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" ref="E4:E52" si="0">CONCATENATE("go playGames(",A4,",",B4,",",C4,",",D4,", 10, TRUE)")</f>
+        <v>go playGames(6,1,5,3, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,3,4,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,3,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="C7">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(4,1,2,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
       <c r="C8">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,2,4,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,1,3,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
       <c r="C10">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,5,8, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,4,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
       <c r="C12">
-        <v>188.1</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,4,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
       <c r="C13">
-        <v>16.690000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,3,6,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="C14">
-        <v>11.05</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,2,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
       <c r="C15">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,2,3,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,3,3, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="C17">
-        <v>224.1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,6,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
       <c r="C18">
-        <v>19.89</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,5,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
       <c r="C19">
-        <v>13.17</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,2,4,3, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
       <c r="C20">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,2,2,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,5,3, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
       <c r="C22">
-        <v>224.1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,2,5,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
       <c r="C23">
-        <v>19.89</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,5,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
       <c r="C24">
-        <v>13.17</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,3,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
       <c r="C25">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,1,2,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,3,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
       <c r="C27">
-        <v>224.1</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,2,4,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
       <c r="C28">
-        <v>19.89</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,3,3,8, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
       <c r="C29">
-        <v>13.17</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,2,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
       <c r="C30">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,2,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,2,3,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
       <c r="C32">
-        <v>224.1</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,2,3,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
       <c r="C33">
-        <v>19.89</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,1,3,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
       <c r="C34">
-        <v>13.17</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,5,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
       <c r="C35">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,1,5,8, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,4,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
       <c r="C37">
-        <v>260.10000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,2,3,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
       <c r="C38">
-        <v>23.08</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,2,3,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
       <c r="C39">
-        <v>15.28</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,1,4,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
       <c r="C40">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,6,8, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,5,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
       <c r="C42">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,3,8, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
       <c r="C43">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,3,7, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
       <c r="C44">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,2,4,8, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
       <c r="C45">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,4,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,1,2,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
       <c r="C47">
-        <v>197.1</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,3,3,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
       <c r="C48">
-        <v>17.489999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,2,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
       <c r="C49">
-        <v>11.58</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,4,4, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
       <c r="C50">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(5,1,3,5, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(6,1,5,6, 10, TRUE)</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
       <c r="C52">
-        <v>18.649999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54">
-        <v>233.1</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55">
-        <v>20.69</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3">
-      <c r="C56">
-        <v>13.69</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3">
-      <c r="C57">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3">
-      <c r="C59">
-        <v>233.1</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3">
-      <c r="C60">
-        <v>20.69</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3">
-      <c r="C61">
-        <v>13.69</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3">
-      <c r="C62">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3">
-      <c r="C64">
-        <v>215.1</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3">
-      <c r="C65">
-        <v>19.09</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3">
-      <c r="C66">
-        <v>12.64</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3">
-      <c r="C67">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3">
-      <c r="C69">
-        <v>242.1</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3">
-      <c r="C70">
-        <v>21.49</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3">
-      <c r="C71">
-        <v>14.22</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3">
-      <c r="C72">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3">
-      <c r="C74">
-        <v>278.10000000000002</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3">
-      <c r="C75">
-        <v>24.68</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3">
-      <c r="C76">
-        <v>16.34</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3">
-      <c r="C77">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="79" spans="3:3">
-      <c r="C79">
-        <v>188.1</v>
-      </c>
-    </row>
-    <row r="80" spans="3:3">
-      <c r="C80">
-        <v>16.690000000000001</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3">
-      <c r="C81">
-        <v>11.05</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3">
-      <c r="C82">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3">
-      <c r="C84">
-        <v>215.1</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3">
-      <c r="C85">
-        <v>19.09</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3">
-      <c r="C86">
-        <v>12.64</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3">
-      <c r="C87">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="89" spans="3:3">
-      <c r="C89">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" spans="3:3">
-      <c r="C91">
-        <v>269.10000000000002</v>
-      </c>
-    </row>
-    <row r="92" spans="3:3">
-      <c r="C92">
-        <v>23.88</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3">
-      <c r="C93">
-        <v>15.81</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3">
-      <c r="C94">
-        <v>3.5</v>
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(7,3,2,5, 10, TRUE)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work in progress on holes
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="4300" windowWidth="24060" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +127,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -137,7 +143,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="615">
+  <cellStyleXfs count="619">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -753,8 +759,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -779,8 +789,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="615">
+  <cellStyles count="619">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1088,6 +1101,8 @@
     <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1395,6 +1410,8 @@
     <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1726,7 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
@@ -2729,8 +2746,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="H14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2752,11 +2773,11 @@
       </c>
       <c r="S14" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U14" t="str">
         <f t="shared" si="17"/>
@@ -2776,7 +2797,7 @@
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, false, false, true, true, false, false, false, false}</v>
       </c>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
@@ -2795,9 +2816,15 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="F15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2813,15 +2840,15 @@
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="13"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="16"/>
@@ -2845,7 +2872,7 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, true, false, false, false, false, false}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -2864,14 +2891,24 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="F16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="M16" s="12" t="s">
+        <v>0</v>
+      </c>
       <c r="O16" t="str">
         <f t="shared" si="11"/>
         <v>false</v>
@@ -2882,19 +2919,19 @@
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="13"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="17"/>
@@ -2910,11 +2947,11 @@
       </c>
       <c r="X16" t="str">
         <f t="shared" si="20"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, true, true, false, false, false, true}</v>
       </c>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -2932,14 +2969,26 @@
         <v>5</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="E17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="12" t="s">
+        <v>0</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="O17" t="str">
         <f t="shared" si="11"/>
@@ -2947,23 +2996,23 @@
       </c>
       <c r="P17" t="str">
         <f t="shared" si="12"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="13"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="17"/>
@@ -2975,7 +3024,7 @@
       </c>
       <c r="W17" t="str">
         <f t="shared" si="19"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="20"/>
@@ -2983,7 +3032,7 @@
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, true, true, true, true, true, false, false, true, false}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -3389,7 +3438,7 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {false, true, true, true, true, true, false, false, true, false}, {false, false, true, true, true, true, false, false, false, true}, {false, false, true, true, true, false, false, false, false, false}, {false, false, false, false, true, true, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">

</xml_diff>

<commit_message>
in the middle of deep refactoring, not compiled version
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="220" windowWidth="17280" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="18220" yWindow="640" windowWidth="10620" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -137,8 +137,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="679">
+  <cellStyleXfs count="727">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -844,7 +892,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="679">
+  <cellStyles count="727">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1184,6 +1232,30 @@
     <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1523,6 +1595,30 @@
     <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1854,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
@@ -2095,6 +2191,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -2175,13 +2272,18 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -2192,11 +2294,11 @@
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="4"/>
@@ -2224,7 +2326,7 @@
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, false, false, false, false, false, false}</v>
       </c>
       <c r="AF6" s="5"/>
       <c r="AG6" s="7" t="s">
@@ -2262,13 +2364,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2281,7 +2383,7 @@
       </c>
       <c r="P7" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="2"/>
@@ -2289,7 +2391,7 @@
       </c>
       <c r="R7" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="4"/>
@@ -2317,7 +2419,7 @@
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, true, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, false, false, false, false, false, false}</v>
       </c>
       <c r="AF7" s="5"/>
       <c r="AG7" s="7" t="s">
@@ -2353,23 +2455,15 @@
         <v>14</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="O8" t="str">
@@ -2378,15 +2472,15 @@
       </c>
       <c r="P8" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="2"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="4"/>
@@ -2394,15 +2488,15 @@
       </c>
       <c r="T8" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="6"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="7"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="8"/>
@@ -2414,7 +2508,7 @@
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, true, false, false, true, true, true, false, false}</v>
+        <v>{false, false, false, true, false, false, false, false, false, false}</v>
       </c>
       <c r="AF8" s="7" t="s">
         <v>0</v>
@@ -2452,30 +2546,18 @@
         <v>13</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="O9" t="str">
         <f t="shared" si="0"/>
@@ -2483,7 +2565,7 @@
       </c>
       <c r="P9" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="2"/>
@@ -2495,23 +2577,23 @@
       </c>
       <c r="S9" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="6"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="7"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="8"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="9"/>
@@ -2519,7 +2601,7 @@
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, true, true, true, true, true, true, true, false}</v>
+        <v>{false, false, true, true, false, false, false, false, false, false}</v>
       </c>
       <c r="AF9" s="7" t="s">
         <v>0</v>
@@ -2563,27 +2645,13 @@
       <c r="F10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -2598,35 +2666,35 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="6"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="7"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="8"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="9"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, true, true, true, true, true, true, true, true}</v>
+        <v>{false, true, true, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF10" s="7" t="s">
         <v>0</v>
@@ -2670,10 +2738,10 @@
       <c r="F11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
       <c r="I11" s="7" t="s">
         <v>0</v>
       </c>
@@ -2686,9 +2754,7 @@
       <c r="L11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="M11" s="1"/>
       <c r="O11" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -2703,11 +2769,11 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="5"/>
@@ -2727,11 +2793,11 @@
       </c>
       <c r="X11" t="str">
         <f t="shared" si="9"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, true, false, true, true, true, true, true, true}</v>
+        <v>{false, true, true, true, false, true, true, true, true, false}</v>
       </c>
       <c r="AF11" s="7" t="s">
         <v>0</v>
@@ -2766,41 +2832,29 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="2"/>
@@ -2812,7 +2866,7 @@
       </c>
       <c r="S12" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="5"/>
@@ -2820,7 +2874,7 @@
       </c>
       <c r="U12" t="str">
         <f t="shared" si="6"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="7"/>
@@ -2828,15 +2882,15 @@
       </c>
       <c r="W12" t="str">
         <f t="shared" si="8"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="9"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, false, true, true}</v>
+        <v>{false, false, true, true, false, true, false, false, false, false}</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>0</v>
@@ -2894,7 +2948,9 @@
       <c r="J13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L13" s="7" t="s">
         <v>0</v>
       </c>
@@ -2931,7 +2987,7 @@
       </c>
       <c r="V13" t="str">
         <f t="shared" ref="V13:V21" si="18">IF(K13=".","true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" ref="W13:W21" si="19">IF(L13=".","true","false")</f>
@@ -2943,7 +2999,7 @@
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, false, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
@@ -2969,16 +3025,16 @@
       <c r="F14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="K14" s="7" t="s">
         <v>0</v>
       </c>
@@ -3002,7 +3058,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="15"/>
@@ -3014,7 +3070,7 @@
       </c>
       <c r="U14" t="str">
         <f t="shared" si="17"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="18"/>
@@ -3030,7 +3086,7 @@
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, false, true, true, true}</v>
+        <v>{true, true, true, false, true, true, true, true, true, true}</v>
       </c>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
@@ -3050,9 +3106,7 @@
       <c r="D15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="7" t="s">
         <v>0</v>
       </c>
@@ -3069,7 +3123,9 @@
       <c r="K15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="1"/>
+      <c r="L15" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="M15" s="7" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +3135,7 @@
       </c>
       <c r="P15" t="str">
         <f t="shared" si="12"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="13"/>
@@ -3107,7 +3163,7 @@
       </c>
       <c r="W15" t="str">
         <f t="shared" si="19"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="20"/>
@@ -3115,7 +3171,7 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, false, true, false, true}</v>
+        <v>{true, false, true, true, true, true, false, true, true, true}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -3159,7 +3215,9 @@
       <c r="L16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O16" t="str">
         <f t="shared" si="11"/>
         <v>true</v>
@@ -3198,11 +3256,11 @@
       </c>
       <c r="X16" t="str">
         <f t="shared" si="20"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, true, false}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -3225,13 +3283,13 @@
       <c r="E17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="7" t="s">
         <v>0</v>
       </c>
@@ -3257,7 +3315,7 @@
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="13"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" si="14"/>
@@ -3265,7 +3323,7 @@
       </c>
       <c r="S17" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="16"/>
@@ -3289,7 +3347,7 @@
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, false, true, true, true, true, true, true, true}</v>
+        <v>{true, true, true, true, false, true, true, true, true, true}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -3318,7 +3376,9 @@
       <c r="G18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="I18" s="7" t="s">
         <v>0</v>
       </c>
@@ -3328,9 +3388,7 @@
       <c r="K18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L18" s="1"/>
       <c r="M18" s="7" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3410,7 @@
       </c>
       <c r="S18" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T18" t="str">
         <f t="shared" si="16"/>
@@ -3368,7 +3426,7 @@
       </c>
       <c r="W18" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X18" t="str">
         <f t="shared" si="20"/>
@@ -3376,7 +3434,7 @@
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, false, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, false, true}</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -3486,9 +3544,7 @@
       <c r="E20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="7" t="s">
         <v>0</v>
       </c>
@@ -3498,7 +3554,9 @@
       <c r="I20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="K20" s="7" t="s">
         <v>0</v>
       </c>
@@ -3518,7 +3576,7 @@
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="13"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="14"/>
@@ -3534,7 +3592,7 @@
       </c>
       <c r="U20" t="str">
         <f t="shared" si="17"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="18"/>
@@ -3550,7 +3608,7 @@
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, false, true, true, true}</v>
+        <v>{true, true, false, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -3579,10 +3637,10 @@
       <c r="G21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1"/>
       <c r="J21" s="7" t="s">
         <v>0</v>
       </c>
@@ -3613,11 +3671,11 @@
       </c>
       <c r="S21" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="17"/>
@@ -3637,7 +3695,7 @@
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, false, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, false, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -3695,7 +3753,7 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, false}, {true, true, true, true, true, true, false, true, false, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, false, true, true}, {false, true, true, false, true, true, true, true, true, true}, {false, true, true, true, true, true, true, true, true, true}, {false, true, true, true, true, true, true, true, true, false}, {false, true, true, false, false, true, true, true, false, false}, {false, true, true, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, true, true, false, true, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, false, true, true, true, true, false, true, true, true}, {true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, false, true, true, false, true, false, false, false, false}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, false, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, true, false, false, false, false, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">

</xml_diff>

<commit_message>
left hole field after tested
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18220" yWindow="640" windowWidth="10620" windowHeight="15080" tabRatio="500"/>
+    <workbookView xWindow="35280" yWindow="10300" windowWidth="12860" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -137,8 +137,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="727">
+  <cellStyleXfs count="763">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -892,7 +928,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="727">
+  <cellStyles count="763">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1256,6 +1292,24 @@
     <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1619,6 +1673,24 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1950,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2373,9 +2445,15 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="J7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="O7" t="str">
         <f t="shared" si="0"/>
@@ -2403,15 +2481,15 @@
       </c>
       <c r="U7" t="str">
         <f t="shared" si="6"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="7"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="8"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="9"/>
@@ -2419,7 +2497,7 @@
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, true, true, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, false, false, true, true, true, false}</v>
       </c>
       <c r="AF7" s="5"/>
       <c r="AG7" s="7" t="s">
@@ -2463,7 +2541,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="O8" t="str">
@@ -2496,7 +2576,7 @@
       </c>
       <c r="V8" t="str">
         <f t="shared" si="7"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="8"/>
@@ -2508,7 +2588,7 @@
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, true, false, false, false, false, false, false}</v>
+        <v>{false, false, false, true, false, false, false, true, false, false}</v>
       </c>
       <c r="AF8" s="7" t="s">
         <v>0</v>
@@ -2556,7 +2636,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="O9" t="str">
@@ -2589,7 +2671,7 @@
       </c>
       <c r="V9" t="str">
         <f t="shared" si="7"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="8"/>
@@ -2601,7 +2683,7 @@
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, true, true, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, false, false, false, true, false, false}</v>
       </c>
       <c r="AF9" s="7" t="s">
         <v>0</v>
@@ -2649,7 +2731,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="O10" t="str">
@@ -2682,7 +2766,7 @@
       </c>
       <c r="V10" t="str">
         <f t="shared" si="7"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="8"/>
@@ -2694,7 +2778,7 @@
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="10"/>
-        <v>{false, true, true, false, false, false, false, false, false, false}</v>
+        <v>{false, true, true, false, false, false, false, true, false, false}</v>
       </c>
       <c r="AF10" s="7" t="s">
         <v>0</v>
@@ -2832,29 +2916,43 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="F12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="I12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="J12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="2"/>
@@ -2866,7 +2964,7 @@
       </c>
       <c r="S12" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="5"/>
@@ -2874,23 +2972,23 @@
       </c>
       <c r="U12" t="str">
         <f t="shared" si="6"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="7"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="8"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="9"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, true, true, false, true, false, false, false, false}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>0</v>
@@ -3025,7 +3123,9 @@
       <c r="F14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="H14" s="7" t="s">
         <v>0</v>
       </c>
@@ -3058,7 +3158,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="15"/>
@@ -3086,7 +3186,7 @@
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, false, true, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
@@ -3106,7 +3206,9 @@
       <c r="D15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="F15" s="7" t="s">
         <v>0</v>
       </c>
@@ -3119,7 +3221,9 @@
       <c r="I15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="K15" s="7" t="s">
         <v>0</v>
       </c>
@@ -3135,7 +3239,7 @@
       </c>
       <c r="P15" t="str">
         <f t="shared" si="12"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="13"/>
@@ -3155,7 +3259,7 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="17"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="18"/>
@@ -3171,7 +3275,7 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="10"/>
-        <v>{true, false, true, true, true, true, false, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -3289,7 +3393,9 @@
       <c r="G17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="I17" s="7" t="s">
         <v>0</v>
       </c>
@@ -3323,7 +3429,7 @@
       </c>
       <c r="S17" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="16"/>
@@ -3347,7 +3453,7 @@
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, false, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -3388,7 +3494,9 @@
       <c r="K18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="1"/>
+      <c r="L18" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="M18" s="7" t="s">
         <v>0</v>
       </c>
@@ -3426,7 +3534,7 @@
       </c>
       <c r="W18" t="str">
         <f t="shared" si="19"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X18" t="str">
         <f t="shared" si="20"/>
@@ -3434,7 +3542,7 @@
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, false, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -3472,7 +3580,9 @@
       <c r="J19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L19" s="7" t="s">
         <v>0</v>
       </c>
@@ -3509,7 +3619,7 @@
       </c>
       <c r="V19" t="str">
         <f t="shared" si="18"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="19"/>
@@ -3521,7 +3631,7 @@
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, false, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -3544,7 +3654,9 @@
       <c r="E20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G20" s="7" t="s">
         <v>0</v>
       </c>
@@ -3576,7 +3688,7 @@
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="13"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="14"/>
@@ -3608,7 +3720,7 @@
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, false, true, true, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -3640,7 +3752,9 @@
       <c r="H21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="J21" s="7" t="s">
         <v>0</v>
       </c>
@@ -3675,7 +3789,7 @@
       </c>
       <c r="T21" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="17"/>
@@ -3695,7 +3809,7 @@
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, false, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -3753,7 +3867,7 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, true, true, true, true, false, true, true, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, false, true, true, true, true, false, true, true, true}, {true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, false, true, true, false, true, false, false, false, false}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, false, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, true, false, false, false, false, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, true, false, false}, {false, false, true, true, false, false, false, true, false, false}, {false, false, false, true, false, false, false, true, false, false}, {false, false, true, true, false, false, true, true, true, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">

</xml_diff>

<commit_message>
excel to test rotation and path
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35280" yWindow="10300" windowWidth="12860" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="13540" yWindow="180" windowWidth="12860" windowHeight="16960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -137,8 +137,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="763">
+  <cellStyleXfs count="837">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -928,7 +1002,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="763">
+  <cellStyles count="837">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1310,6 +1384,43 @@
     <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1691,6 +1802,43 @@
     <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2022,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2043,10 +2191,18 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -2064,19 +2220,19 @@
       </c>
       <c r="R2" t="str">
         <f t="shared" ref="R2:R12" si="3">IF(G2=".","true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S2" t="str">
         <f t="shared" ref="S2:S12" si="4">IF(H2=".","true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T2" t="str">
         <f t="shared" ref="T2:T12" si="5">IF(I2=".","true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U2" t="str">
         <f t="shared" ref="U2:U12" si="6">IF(J2=".","true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V2" t="str">
         <f t="shared" ref="V2:V12" si="7">IF(K2=".","true","false")</f>
@@ -2092,7 +2248,7 @@
       </c>
       <c r="Z2" t="str">
         <f>CONCATENATE("{",O2,", ",P2,", ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", ",V2,", ",W2,", ",X2,"}")</f>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, false, true, true, true, true, false, false, false}</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="27" customHeight="1">
@@ -2101,7 +2257,9 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2118,7 +2276,7 @@
       </c>
       <c r="Q3" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="3"/>
@@ -2150,7 +2308,7 @@
       </c>
       <c r="Z3" t="str">
         <f t="shared" ref="Z3:Z21" si="10">CONCATENATE("{",O3,", ",P3,", ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", ",V3,", ",W3,", ",X3,"}")</f>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="7" t="s">
@@ -2178,13 +2336,17 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O4" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -2195,7 +2357,7 @@
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="3"/>
@@ -2219,7 +2381,7 @@
       </c>
       <c r="W4" t="str">
         <f t="shared" si="8"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X4" t="str">
         <f t="shared" si="9"/>
@@ -2227,7 +2389,7 @@
       </c>
       <c r="Z4" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, false, false, false, false, false, true, false}</v>
       </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="7" t="s">
@@ -2256,13 +2418,17 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
@@ -2274,7 +2440,7 @@
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="3"/>
@@ -2298,7 +2464,7 @@
       </c>
       <c r="W5" t="str">
         <f t="shared" si="8"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="9"/>
@@ -2306,7 +2472,7 @@
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, false, false, false, false, false, true, false}</v>
       </c>
       <c r="AF5" s="5"/>
       <c r="AG5" s="7" t="s">
@@ -2354,7 +2520,9 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
@@ -2390,7 +2558,7 @@
       </c>
       <c r="W6" t="str">
         <f t="shared" si="8"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="9"/>
@@ -2398,7 +2566,7 @@
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="10"/>
-        <v>{false, false, true, true, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, false, false, false, false, true, false}</v>
       </c>
       <c r="AF6" s="5"/>
       <c r="AG6" s="7" t="s">
@@ -3209,9 +3377,7 @@
       <c r="E15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="7" t="s">
         <v>0</v>
       </c>
@@ -3243,7 +3409,7 @@
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="13"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="14"/>
@@ -3275,7 +3441,7 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, true, false, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -3313,9 +3479,7 @@
       <c r="J16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="7" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3516,7 @@
       </c>
       <c r="V16" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="19"/>
@@ -3364,7 +3528,7 @@
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, true, true, false, true, true}</v>
       </c>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -3574,9 +3738,7 @@
       <c r="H19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="I19" s="1"/>
       <c r="J19" s="7" t="s">
         <v>0</v>
       </c>
@@ -3611,7 +3773,7 @@
       </c>
       <c r="T19" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U19" t="str">
         <f t="shared" si="17"/>
@@ -3631,7 +3793,7 @@
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, true, true, true, true, false, true, true, true, true}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -3740,9 +3902,7 @@
       <c r="D21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="7" t="s">
         <v>0</v>
       </c>
@@ -3773,7 +3933,7 @@
       </c>
       <c r="P21" t="str">
         <f t="shared" si="12"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="13"/>
@@ -3809,7 +3969,7 @@
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="10"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, false, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -3867,7 +4027,7 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, true, false, false}, {false, false, true, true, false, false, false, true, false, false}, {false, false, false, true, false, false, false, true, false, false}, {false, false, true, true, false, false, true, true, true, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, false, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, true, false, false}, {false, false, true, true, false, false, false, true, false, false}, {false, false, false, true, false, false, false, true, false, false}, {false, false, true, true, false, false, true, true, true, false}, {false, false, true, true, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, false, true, true, true, true, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">

</xml_diff>

<commit_message>
playing with recursive function
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13540" yWindow="180" windowWidth="12860" windowHeight="16960" tabRatio="500"/>
+    <workbookView xWindow="27760" yWindow="12180" windowWidth="14000" windowHeight="15440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="best strategy compiler" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -56,8 +56,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +113,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -137,842 +147,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="837">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1002,847 +178,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="837">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="767" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="769" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="771" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="773" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -2167,45 +509,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:AQ40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="13" width="4.83203125" customWidth="1"/>
-    <col min="15" max="24" width="6.5" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="13" width="4.85546875" customWidth="1"/>
+    <col min="15" max="24" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:43">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
     <row r="2" spans="1:43" ht="27" customHeight="1">
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>0</v>
-      </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
       <c r="O2" t="str">
         <f t="shared" ref="O2:O12" si="0">IF(D2=".","true","false")</f>
         <v>false</v>
@@ -2215,40 +551,40 @@
         <v>false</v>
       </c>
       <c r="Q2" t="str">
-        <f t="shared" ref="Q2:Q12" si="2">IF(F2=".","true","false")</f>
+        <f t="shared" ref="Q2" si="2">IF(F2=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="R2" t="str">
-        <f t="shared" ref="R2:R12" si="3">IF(G2=".","true","false")</f>
-        <v>true</v>
+        <f>IF(G2=".","true","false")</f>
+        <v>false</v>
       </c>
       <c r="S2" t="str">
-        <f t="shared" ref="S2:S12" si="4">IF(H2=".","true","false")</f>
-        <v>true</v>
+        <f>IF(H2=".","true","false")</f>
+        <v>false</v>
       </c>
       <c r="T2" t="str">
-        <f t="shared" ref="T2:T12" si="5">IF(I2=".","true","false")</f>
-        <v>true</v>
+        <f>IF(I2=".","true","false")</f>
+        <v>false</v>
       </c>
       <c r="U2" t="str">
-        <f t="shared" ref="U2:U12" si="6">IF(J2=".","true","false")</f>
-        <v>true</v>
+        <f>IF(J2=".","true","false")</f>
+        <v>false</v>
       </c>
       <c r="V2" t="str">
-        <f t="shared" ref="V2:V12" si="7">IF(K2=".","true","false")</f>
+        <f>IF(K2=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="W2" t="str">
-        <f t="shared" ref="W2:W12" si="8">IF(L2=".","true","false")</f>
+        <f>IF(L2=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="X2" t="str">
-        <f t="shared" ref="X2:X12" si="9">IF(M2=".","true","false")</f>
+        <f>IF(M2=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="Z2" t="str">
-        <f>CONCATENATE("{",O2,", ",P2,", ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", ",V2,", ",W2,", ",X2,"}")</f>
-        <v>{false, false, false, true, true, true, true, false, false, false}</v>
+        <f t="shared" ref="Z2:Z21" si="3">CONCATENATE("{",O2,", ",P2,", ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", ",V2,", ",W2,", ",X2,"}")</f>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="27" customHeight="1">
@@ -2275,39 +611,39 @@
         <v>false</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="Q2:Q12" si="4">IF(F3=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="R3" t="str">
+        <f>IF(G3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="S3" t="str">
+        <f>IF(H3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="T3" t="str">
+        <f>IF(I3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="U3" t="str">
+        <f>IF(J3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="V3" t="str">
+        <f>IF(K3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="W3" t="str">
+        <f>IF(L3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="X3" t="str">
+        <f>IF(M3=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="Z3" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
-      </c>
-      <c r="S3" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T3" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U3" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V3" t="str">
-        <f t="shared" si="7"/>
-        <v>false</v>
-      </c>
-      <c r="W3" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="X3" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z21" si="10">CONCATENATE("{",O3,", ",P3,", ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", ",V3,", ",W3,", ",X3,"}")</f>
         <v>{false, false, true, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF3" s="5"/>
@@ -2339,7 +675,9 @@
       <c r="F4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2356,40 +694,40 @@
         <v>false</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R4" t="str">
+        <f>IF(G4=".","true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="S4" t="str">
+        <f>IF(H4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="T4" t="str">
+        <f>IF(I4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="U4" t="str">
+        <f>IF(J4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="V4" t="str">
+        <f>IF(K4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" ref="W4:W12" si="5">IF(L4=".","true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" ref="X4:X12" si="6">IF(M4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="Z4" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
-      </c>
-      <c r="S4" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T4" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U4" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V4" t="str">
-        <f t="shared" si="7"/>
-        <v>false</v>
-      </c>
-      <c r="W4" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="X4" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z4" t="str">
-        <f t="shared" si="10"/>
-        <v>{false, false, true, false, false, false, false, false, true, false}</v>
+        <v>{false, false, true, true, false, false, false, false, true, false}</v>
       </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="7" t="s">
@@ -2439,39 +777,39 @@
         <v>false</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R5" t="str">
+        <f>IF(G5=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="S5" t="str">
+        <f>IF(H5=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="T5" t="str">
+        <f>IF(I5=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="U5" t="str">
+        <f>IF(J5=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="V5" t="str">
+        <f>IF(K5=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="X5" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z5" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
-      </c>
-      <c r="S5" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T5" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U5" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V5" t="str">
-        <f t="shared" si="7"/>
-        <v>false</v>
-      </c>
-      <c r="W5" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="X5" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z5" t="str">
-        <f t="shared" si="10"/>
         <v>{false, false, true, false, false, false, false, false, true, false}</v>
       </c>
       <c r="AF5" s="5"/>
@@ -2533,39 +871,39 @@
         <v>false</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R6" t="str">
+        <f t="shared" ref="R6:R12" si="7">IF(G6=".","true","false")</f>
+        <v>true</v>
+      </c>
+      <c r="S6" t="str">
+        <f>IF(H6=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="T6" t="str">
+        <f>IF(I6=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" ref="U6:U12" si="8">IF(J6=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" ref="V6:V12" si="9">IF(K6=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z6" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
-      </c>
-      <c r="S6" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T6" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V6" t="str">
-        <f t="shared" si="7"/>
-        <v>false</v>
-      </c>
-      <c r="W6" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="10"/>
         <v>{false, false, true, true, false, false, false, false, true, false}</v>
       </c>
       <c r="AF6" s="5"/>
@@ -2632,39 +970,39 @@
         <v>false</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R7" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" ref="S7:S12" si="10">IF(H7=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" ref="T7:T12" si="11">IF(I7=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="8"/>
+        <v>true</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="9"/>
+        <v>true</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z7" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
-      </c>
-      <c r="S7" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T7" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="6"/>
-        <v>true</v>
-      </c>
-      <c r="V7" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="W7" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="X7" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="10"/>
         <v>{false, false, true, true, false, false, true, true, true, false}</v>
       </c>
       <c r="AF7" s="5"/>
@@ -2723,39 +1061,39 @@
         <v>false</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>false</v>
       </c>
       <c r="R8" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="9"/>
+        <v>true</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z8" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
-      </c>
-      <c r="S8" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T8" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V8" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="W8" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="10"/>
         <v>{false, false, false, true, false, false, false, true, false, false}</v>
       </c>
       <c r="AF8" s="7" t="s">
@@ -2804,9 +1142,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="O9" t="str">
@@ -2818,40 +1154,40 @@
         <v>false</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R9" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="9"/>
+        <v>false</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z9" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
-      </c>
-      <c r="S9" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T9" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U9" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V9" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="W9" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="X9" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z9" t="str">
-        <f t="shared" si="10"/>
-        <v>{false, false, true, true, false, false, false, true, false, false}</v>
+        <v>{false, false, true, true, false, false, false, false, false, false}</v>
       </c>
       <c r="AF9" s="7" t="s">
         <v>0</v>
@@ -2913,39 +1249,39 @@
         <v>true</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R10" t="str">
+        <f t="shared" si="7"/>
+        <v>false</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="9"/>
+        <v>true</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z10" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
-      </c>
-      <c r="S10" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T10" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="V10" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="W10" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="10"/>
         <v>{false, true, true, false, false, false, false, true, false, false}</v>
       </c>
       <c r="AF10" s="7" t="s">
@@ -3016,39 +1352,39 @@
         <v>true</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R11" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="11"/>
+        <v>true</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="8"/>
+        <v>true</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="9"/>
+        <v>true</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="Z11" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
-      </c>
-      <c r="S11" t="str">
-        <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="T11" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="U11" t="str">
-        <f t="shared" si="6"/>
-        <v>true</v>
-      </c>
-      <c r="V11" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="W11" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="X11" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="Z11" t="str">
-        <f t="shared" si="10"/>
         <v>{false, true, true, true, false, true, true, true, true, false}</v>
       </c>
       <c r="AF11" s="7" t="s">
@@ -3123,39 +1459,39 @@
         <v>true</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="R12" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="10"/>
+        <v>true</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="11"/>
+        <v>true</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="8"/>
+        <v>true</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="9"/>
+        <v>true</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="X12" t="str">
+        <f t="shared" si="6"/>
+        <v>true</v>
+      </c>
+      <c r="Z12" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
-      </c>
-      <c r="S12" t="str">
-        <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="T12" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="U12" t="str">
-        <f t="shared" si="6"/>
-        <v>true</v>
-      </c>
-      <c r="V12" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="W12" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="X12" t="str">
-        <f t="shared" si="9"/>
-        <v>true</v>
-      </c>
-      <c r="Z12" t="str">
-        <f t="shared" si="10"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AF12" s="7" t="s">
@@ -3224,47 +1560,47 @@
         <v>0</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" ref="O13:O21" si="11">IF(D13=".","true","false")</f>
+        <f t="shared" ref="O13:O21" si="12">IF(D13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" ref="P13:P21" si="12">IF(E13=".","true","false")</f>
+        <f t="shared" ref="P13:P21" si="13">IF(E13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" ref="Q13:Q21" si="13">IF(F13=".","true","false")</f>
+        <f t="shared" ref="Q13:Q21" si="14">IF(F13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" ref="R13:R21" si="14">IF(G13=".","true","false")</f>
+        <f t="shared" ref="R13:R21" si="15">IF(G13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" ref="S13:S21" si="15">IF(H13=".","true","false")</f>
+        <f t="shared" ref="S13:S21" si="16">IF(H13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" ref="T13:T21" si="16">IF(I13=".","true","false")</f>
+        <f t="shared" ref="T13:T21" si="17">IF(I13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="U13" t="str">
-        <f t="shared" ref="U13:U21" si="17">IF(J13=".","true","false")</f>
+        <f t="shared" ref="U13:U21" si="18">IF(J13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="V13" t="str">
-        <f t="shared" ref="V13:V21" si="18">IF(K13=".","true","false")</f>
+        <f t="shared" ref="V13:V21" si="19">IF(K13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="W13" t="str">
-        <f t="shared" ref="W13:W21" si="19">IF(L13=".","true","false")</f>
+        <f t="shared" ref="W13:W21" si="20">IF(L13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="X13" t="str">
-        <f t="shared" ref="X13:X21" si="20">IF(M13=".","true","false")</f>
+        <f t="shared" ref="X13:X21" si="21">IF(M13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH13" s="6"/>
@@ -3313,47 +1649,47 @@
         <v>0</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U14" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V14" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W14" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X14" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH14" s="6"/>
@@ -3400,47 +1736,47 @@
         <v>0</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>false</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V15" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X15" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, false, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH15" s="6"/>
@@ -3487,47 +1823,47 @@
         <v>0</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V16" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>false</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, true, true, false, true, true}</v>
       </c>
       <c r="AH16" s="6"/>
@@ -3576,47 +1912,47 @@
         <v>0</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V17" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X17" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH17" s="6"/>
@@ -3665,47 +2001,47 @@
         <v>0</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X18" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH18" s="6"/>
@@ -3752,47 +2088,47 @@
         <v>0</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>false</v>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V19" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X19" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, false, true, true, true, true}</v>
       </c>
       <c r="AH19" s="6"/>
@@ -3841,47 +2177,47 @@
         <v>0</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>true</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH20" s="6"/>
@@ -3928,47 +2264,47 @@
         <v>0</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>true</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>false</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>{true, false, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
@@ -4027,17 +2363,19 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, false, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, true, false, false}, {false, false, true, true, false, false, false, true, false, false}, {false, false, false, true, false, false, false, true, false, false}, {false, false, true, true, false, false, true, true, true, false}, {false, false, true, true, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, false, true, true, true, true, false, false, false}}</v>
+        <v>{{true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, false, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, true, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, true, false, false, false, true, false, false}, {false, false, true, true, false, false, true, true, true, false}, {false, false, true, true, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, true, false}, {false, false, true, true, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">
       <c r="G40" s="4"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -4045,18 +2383,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="C2:E12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="25"/>
   <cols>
     <col min="3" max="3" width="59" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5">
@@ -4106,10 +2445,10 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -4117,16 +2456,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="42.83203125" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
@@ -5030,10 +3370,10 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Drop on empty rows increase performance 5 time
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="10">
   <si>
     <t>.</t>
   </si>
@@ -513,16 +513,13 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="13" width="4.85546875" customWidth="1"/>
+    <col min="1" max="13" width="4.28515625" customWidth="1"/>
     <col min="15" max="24" width="6.42578125" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="10.140625" customWidth="1"/>
   </cols>
@@ -555,35 +552,35 @@
         <v>false</v>
       </c>
       <c r="R2" t="str">
-        <f>IF(G2=".","true","false")</f>
+        <f t="shared" ref="R2:X3" si="3">IF(G2=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="S2" t="str">
-        <f>IF(H2=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="T2" t="str">
-        <f>IF(I2=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="U2" t="str">
-        <f>IF(J2=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="V2" t="str">
-        <f>IF(K2=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="W2" t="str">
-        <f>IF(L2=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="X2" t="str">
-        <f>IF(M2=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="Z2" t="str">
-        <f t="shared" ref="Z2:Z21" si="3">CONCATENATE("{",O2,", ",P2,", ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", ",V2,", ",W2,", ",X2,"}")</f>
+        <f t="shared" ref="Z2:Z21" si="4">CONCATENATE("{",O2,", ",P2,", ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", ",V2,", ",W2,", ",X2,"}")</f>
         <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
     </row>
@@ -593,15 +590,14 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
       <c r="O3" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -611,40 +607,40 @@
         <v>false</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q2:Q12" si="4">IF(F3=".","true","false")</f>
-        <v>true</v>
+        <f t="shared" ref="Q3:Q12" si="5">IF(F3=".","true","false")</f>
+        <v>false</v>
       </c>
       <c r="R3" t="str">
-        <f>IF(G3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="S3" t="str">
-        <f>IF(H3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="T3" t="str">
-        <f>IF(I3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="U3" t="str">
-        <f>IF(J3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="V3" t="str">
-        <f>IF(K3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="W3" t="str">
-        <f>IF(L3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="X3" t="str">
-        <f>IF(M3=".","true","false")</f>
+        <f t="shared" si="3"/>
         <v>false</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, true, false, false, false, false, false, false, false}</v>
+        <f t="shared" si="4"/>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="7" t="s">
@@ -672,19 +668,14 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
       <c r="O4" t="str">
         <f t="shared" si="0"/>
         <v>false</v>
@@ -694,40 +685,40 @@
         <v>false</v>
       </c>
       <c r="Q4" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" ref="R4:V5" si="6">IF(G4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" ref="W4:W12" si="7">IF(L4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" ref="X4:X12" si="8">IF(M4=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="Z4" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R4" t="str">
-        <f>IF(G4=".","true","false")</f>
-        <v>true</v>
-      </c>
-      <c r="S4" t="str">
-        <f>IF(H4=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="T4" t="str">
-        <f>IF(I4=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="U4" t="str">
-        <f>IF(J4=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="V4" t="str">
-        <f>IF(K4=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="W4" t="str">
-        <f t="shared" ref="W4:W12" si="5">IF(L4=".","true","false")</f>
-        <v>true</v>
-      </c>
-      <c r="X4" t="str">
-        <f t="shared" ref="X4:X12" si="6">IF(M4=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="Z4" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, true, true, false, false, false, false, true, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="7" t="s">
@@ -756,17 +747,13 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
@@ -777,40 +764,40 @@
         <v>false</v>
       </c>
       <c r="Q5" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="R5" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="7"/>
+        <v>false</v>
+      </c>
+      <c r="X5" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="Z5" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R5" t="str">
-        <f>IF(G5=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="S5" t="str">
-        <f>IF(H5=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="T5" t="str">
-        <f>IF(I5=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="U5" t="str">
-        <f>IF(J5=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="V5" t="str">
-        <f>IF(K5=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="W5" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="X5" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="Z5" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, true, false, false, false, false, false, true, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF5" s="5"/>
       <c r="AG5" s="7" t="s">
@@ -848,19 +835,13 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
@@ -871,12 +852,12 @@
         <v>false</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="4"/>
-        <v>true</v>
+        <f t="shared" si="5"/>
+        <v>false</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" ref="R6:R12" si="7">IF(G6=".","true","false")</f>
-        <v>true</v>
+        <f t="shared" ref="R6:R12" si="9">IF(G6=".","true","false")</f>
+        <v>false</v>
       </c>
       <c r="S6" t="str">
         <f>IF(H6=".","true","false")</f>
@@ -887,24 +868,24 @@
         <v>false</v>
       </c>
       <c r="U6" t="str">
-        <f t="shared" ref="U6:U12" si="8">IF(J6=".","true","false")</f>
+        <f t="shared" ref="U6:U12" si="10">IF(J6=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="V6" t="str">
-        <f t="shared" ref="V6:V12" si="9">IF(K6=".","true","false")</f>
+        <f t="shared" ref="V6:V12" si="11">IF(K6=".","true","false")</f>
         <v>false</v>
       </c>
       <c r="W6" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
+        <f t="shared" si="7"/>
+        <v>false</v>
       </c>
       <c r="X6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>false</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, true, true, false, false, false, false, true, false}</v>
+        <f t="shared" si="4"/>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF6" s="5"/>
       <c r="AG6" s="7" t="s">
@@ -943,23 +924,13 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="O7" t="str">
         <f t="shared" si="0"/>
@@ -970,40 +941,40 @@
         <v>false</v>
       </c>
       <c r="Q7" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="9"/>
+        <v>false</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" ref="S7:S12" si="12">IF(H7=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" ref="T7:T12" si="13">IF(I7=".","true","false")</f>
+        <v>false</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="7"/>
+        <v>false</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="Z7" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R7" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="S7" t="str">
-        <f t="shared" ref="S7:S12" si="10">IF(H7=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="T7" t="str">
-        <f t="shared" ref="T7:T12" si="11">IF(I7=".","true","false")</f>
-        <v>false</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="V7" t="str">
-        <f t="shared" si="9"/>
-        <v>true</v>
-      </c>
-      <c r="W7" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="X7" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, true, true, false, false, true, true, true, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF7" s="5"/>
       <c r="AG7" s="7" t="s">
@@ -1041,15 +1012,11 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="O8" t="str">
@@ -1061,40 +1028,40 @@
         <v>false</v>
       </c>
       <c r="Q8" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="9"/>
+        <v>false</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="12"/>
+        <v>false</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="13"/>
+        <v>false</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="7"/>
+        <v>false</v>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="Z8" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="S8" t="str">
-        <f t="shared" si="10"/>
-        <v>false</v>
-      </c>
-      <c r="T8" t="str">
-        <f t="shared" si="11"/>
-        <v>false</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="V8" t="str">
-        <f t="shared" si="9"/>
-        <v>true</v>
-      </c>
-      <c r="W8" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, false, true, false, false, false, true, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF8" s="7" t="s">
         <v>0</v>
@@ -1133,12 +1100,8 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1154,40 +1117,40 @@
         <v>false</v>
       </c>
       <c r="Q9" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="9"/>
+        <v>false</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="12"/>
+        <v>false</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="13"/>
+        <v>false</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="7"/>
+        <v>false</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="Z9" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R9" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="S9" t="str">
-        <f t="shared" si="10"/>
-        <v>false</v>
-      </c>
-      <c r="T9" t="str">
-        <f t="shared" si="11"/>
-        <v>false</v>
-      </c>
-      <c r="U9" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="V9" t="str">
-        <f t="shared" si="9"/>
-        <v>false</v>
-      </c>
-      <c r="W9" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="X9" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="Z9" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, false, true, true, false, false, false, false, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF9" s="7" t="s">
         <v>0</v>
@@ -1225,19 +1188,13 @@
         <v>12</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="O10" t="str">
@@ -1246,43 +1203,43 @@
       </c>
       <c r="P10" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q10" t="str">
+        <f t="shared" si="5"/>
+        <v>false</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="9"/>
+        <v>false</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="12"/>
+        <v>false</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="13"/>
+        <v>false</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="7"/>
+        <v>false</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="Z10" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" si="7"/>
-        <v>false</v>
-      </c>
-      <c r="S10" t="str">
-        <f t="shared" si="10"/>
-        <v>false</v>
-      </c>
-      <c r="T10" t="str">
-        <f t="shared" si="11"/>
-        <v>false</v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="8"/>
-        <v>false</v>
-      </c>
-      <c r="V10" t="str">
-        <f t="shared" si="9"/>
-        <v>true</v>
-      </c>
-      <c r="W10" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, true, true, false, false, false, false, true, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF10" s="7" t="s">
         <v>0</v>
@@ -1320,25 +1277,15 @@
         <v>11</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1349,43 +1296,43 @@
       </c>
       <c r="P11" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q11" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="9"/>
+        <v>false</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="12"/>
+        <v>false</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="13"/>
+        <v>false</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="8"/>
+        <v>false</v>
+      </c>
+      <c r="Z11" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="S11" t="str">
-        <f t="shared" si="10"/>
-        <v>false</v>
-      </c>
-      <c r="T11" t="str">
-        <f t="shared" si="11"/>
-        <v>true</v>
-      </c>
-      <c r="U11" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="V11" t="str">
-        <f t="shared" si="9"/>
-        <v>true</v>
-      </c>
-      <c r="W11" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="X11" t="str">
-        <f t="shared" si="6"/>
-        <v>false</v>
-      </c>
-      <c r="Z11" t="str">
-        <f t="shared" si="3"/>
-        <v>{false, true, true, true, false, true, true, true, true, false}</v>
+        <v>{false, false, true, false, false, false, false, false, true, false}</v>
       </c>
       <c r="AF11" s="7" t="s">
         <v>0</v>
@@ -1423,9 +1370,7 @@
       <c r="D12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="7" t="s">
         <v>0</v>
       </c>
@@ -1435,15 +1380,9 @@
       <c r="H12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
       <c r="L12" s="7" t="s">
         <v>0</v>
       </c>
@@ -1456,43 +1395,43 @@
       </c>
       <c r="P12" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q12" t="str">
+        <f t="shared" si="5"/>
+        <v>true</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="9"/>
+        <v>true</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="12"/>
+        <v>true</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="13"/>
+        <v>false</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="10"/>
+        <v>false</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="11"/>
+        <v>false</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="7"/>
+        <v>true</v>
+      </c>
+      <c r="X12" t="str">
+        <f t="shared" si="8"/>
+        <v>true</v>
+      </c>
+      <c r="Z12" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
-      </c>
-      <c r="R12" t="str">
-        <f t="shared" si="7"/>
-        <v>true</v>
-      </c>
-      <c r="S12" t="str">
-        <f t="shared" si="10"/>
-        <v>true</v>
-      </c>
-      <c r="T12" t="str">
-        <f t="shared" si="11"/>
-        <v>true</v>
-      </c>
-      <c r="U12" t="str">
-        <f t="shared" si="8"/>
-        <v>true</v>
-      </c>
-      <c r="V12" t="str">
-        <f t="shared" si="9"/>
-        <v>true</v>
-      </c>
-      <c r="W12" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="X12" t="str">
-        <f t="shared" si="6"/>
-        <v>true</v>
-      </c>
-      <c r="Z12" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, false, true, true, true, false, false, false, true, true}</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>0</v>
@@ -1541,13 +1480,13 @@
       <c r="G13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="H13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="K13" s="7" t="s">
@@ -1560,47 +1499,47 @@
         <v>0</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" ref="O13:O21" si="12">IF(D13=".","true","false")</f>
+        <f t="shared" ref="O13:O21" si="14">IF(D13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" ref="P13:P21" si="13">IF(E13=".","true","false")</f>
+        <f t="shared" ref="P13:P21" si="15">IF(E13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" ref="Q13:Q21" si="14">IF(F13=".","true","false")</f>
+        <f t="shared" ref="Q13:Q21" si="16">IF(F13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" ref="R13:R21" si="15">IF(G13=".","true","false")</f>
+        <f t="shared" ref="R13:R21" si="17">IF(G13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" ref="S13:S21" si="16">IF(H13=".","true","false")</f>
+        <f t="shared" ref="S13:S21" si="18">IF(H13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" ref="T13:T21" si="17">IF(I13=".","true","false")</f>
+        <f t="shared" ref="T13:T21" si="19">IF(I13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="U13" t="str">
-        <f t="shared" ref="U13:U21" si="18">IF(J13=".","true","false")</f>
+        <f t="shared" ref="U13:U21" si="20">IF(J13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="V13" t="str">
-        <f t="shared" ref="V13:V21" si="19">IF(K13=".","true","false")</f>
+        <f t="shared" ref="V13:V21" si="21">IF(K13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="W13" t="str">
-        <f t="shared" ref="W13:W21" si="20">IF(L13=".","true","false")</f>
+        <f t="shared" ref="W13:W21" si="22">IF(L13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="X13" t="str">
-        <f t="shared" ref="X13:X21" si="21">IF(M13=".","true","false")</f>
+        <f t="shared" ref="X13:X21" si="23">IF(M13=".","true","false")</f>
         <v>true</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH13" s="6"/>
@@ -1633,7 +1572,7 @@
       <c r="H14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="7" t="s">
@@ -1649,47 +1588,47 @@
         <v>0</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U14" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V14" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="W14" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X14" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>{true, true, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH14" s="6"/>
@@ -1713,7 +1652,9 @@
       <c r="E15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1723,9 +1664,7 @@
       <c r="I15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1736,48 +1675,48 @@
         <v>0</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="14"/>
-        <v>false</v>
+        <f t="shared" si="16"/>
+        <v>true</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="18"/>
-        <v>true</v>
+        <f t="shared" si="20"/>
+        <v>false</v>
       </c>
       <c r="V15" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X15" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, false, true, true, true, true, true, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, true, true, true, true, true, false, true, true, true}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -1797,9 +1736,7 @@
       <c r="D16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="7" t="s">
         <v>0</v>
       </c>
@@ -1815,7 +1752,9 @@
       <c r="J16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="L16" s="7" t="s">
         <v>0</v>
       </c>
@@ -1823,48 +1762,48 @@
         <v>0</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="13"/>
-        <v>true</v>
+        <f t="shared" si="15"/>
+        <v>false</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V16" t="str">
-        <f t="shared" si="19"/>
-        <v>false</v>
+        <f t="shared" si="21"/>
+        <v>true</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X16" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, true, true, true, true, true, false, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, false, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -1908,52 +1847,50 @@
       <c r="L17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M17" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="M17" s="1"/>
       <c r="O17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V17" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X17" t="str">
-        <f t="shared" si="21"/>
-        <v>true</v>
+        <f t="shared" si="23"/>
+        <v>false</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, true, true, true, true, true, true, true, true, false}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -1991,9 +1928,7 @@
       <c r="J18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K18" s="1"/>
       <c r="L18" s="7" t="s">
         <v>0</v>
       </c>
@@ -2001,48 +1936,48 @@
         <v>0</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V18" t="str">
-        <f t="shared" si="19"/>
-        <v>true</v>
+        <f t="shared" si="21"/>
+        <v>false</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, true, true, true, true, true, true, false, true, true}</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -2074,62 +2009,62 @@
       <c r="H19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="J19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L19" s="1"/>
       <c r="M19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="17"/>
-        <v>false</v>
+        <f t="shared" si="19"/>
+        <v>true</v>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="20"/>
-        <v>true</v>
+        <f t="shared" si="22"/>
+        <v>false</v>
       </c>
       <c r="X19" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, true, true, true, false, true, true, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, true, true, true, true, true, true, true, false, true}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -2158,9 +2093,7 @@
       <c r="G20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H20" s="1"/>
       <c r="I20" s="7" t="s">
         <v>0</v>
       </c>
@@ -2177,48 +2110,48 @@
         <v>0</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>true</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>true</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="16"/>
-        <v>true</v>
+        <f t="shared" si="18"/>
+        <v>false</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, true, true, true, false, true, true, true, true, true}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -2238,13 +2171,13 @@
       <c r="D21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="F21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="7" t="s">
         <v>0</v>
       </c>
@@ -2264,48 +2197,48 @@
         <v>0</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>true</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="13"/>
-        <v>false</v>
+        <f t="shared" si="15"/>
+        <v>true</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>true</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="15"/>
-        <v>true</v>
+        <f t="shared" si="17"/>
+        <v>false</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>true</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>true</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>true</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>true</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>true</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="3"/>
-        <v>{true, false, true, true, true, true, true, true, true, true}</v>
+        <f t="shared" si="4"/>
+        <v>{true, true, true, false, true, true, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -2363,14 +2296,13 @@
     <row r="23" spans="3:43">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, false, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, false, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {false, true, true, true, false, true, true, true, true, false}, {false, true, true, false, false, false, false, true, false, false}, {false, false, true, true, false, false, false, false, false, false}, {false, false, false, true, false, false, false, true, false, false}, {false, false, true, true, false, false, true, true, true, false}, {false, false, true, true, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, true, false}, {false, false, true, true, false, false, false, false, true, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, true, false}, {true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, false, true, true, true, false, false, false, true, true}, {false, false, true, false, false, false, false, false, true, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7">
       <c r="G40" s="4"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2445,7 +2377,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3370,7 +3301,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
After analyzing statistic found a better way to test strategies
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkezlya/go/src/penek/analitics/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27760" yWindow="12180" windowWidth="14000" windowHeight="15440" tabRatio="500"/>
+    <workbookView xWindow="23960" yWindow="7880" windowWidth="19760" windowHeight="18820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="best strategy compiler" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="130000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="15">
   <si>
     <t>.</t>
   </si>
@@ -52,18 +57,27 @@
   <si>
     <t>always check for burn BUG damadge</t>
   </si>
+  <si>
+    <t>Burn</t>
+  </si>
+  <si>
+    <t>BHoles</t>
+  </si>
+  <si>
+    <t>FHoles</t>
+  </si>
+  <si>
+    <t>HighY</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,7 +198,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -509,7 +528,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AQ40"/>
   <sheetViews>
@@ -517,14 +536,14 @@
       <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="4.28515625" customWidth="1"/>
-    <col min="15" max="24" width="6.42578125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" customWidth="1"/>
+    <col min="1" max="13" width="4.33203125" customWidth="1"/>
+    <col min="15" max="24" width="6.5" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -534,7 +553,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:43" ht="27" customHeight="1">
+    <row r="2" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>20</v>
       </c>
@@ -584,7 +603,7 @@
         <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="27" customHeight="1">
+    <row r="3" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>19</v>
       </c>
@@ -659,7 +678,7 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="27" customHeight="1">
+    <row r="4" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -741,7 +760,7 @@
       <c r="AN4" s="11"/>
       <c r="AO4" s="11"/>
     </row>
-    <row r="5" spans="1:43" ht="27" customHeight="1">
+    <row r="5" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>17</v>
       </c>
@@ -826,7 +845,7 @@
       </c>
       <c r="AO5" s="5"/>
     </row>
-    <row r="6" spans="1:43" ht="27" customHeight="1">
+    <row r="6" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -918,7 +937,7 @@
       <c r="AP6" s="3"/>
       <c r="AQ6" s="3"/>
     </row>
-    <row r="7" spans="1:43" ht="27" customHeight="1">
+    <row r="7" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>15</v>
       </c>
@@ -1005,7 +1024,7 @@
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3"/>
     </row>
-    <row r="8" spans="1:43" ht="27" customHeight="1">
+    <row r="8" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>14</v>
       </c>
@@ -1094,7 +1113,7 @@
       <c r="AP8" s="6"/>
       <c r="AQ8" s="6"/>
     </row>
-    <row r="9" spans="1:43" ht="27" customHeight="1">
+    <row r="9" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>13</v>
       </c>
@@ -1183,7 +1202,7 @@
       <c r="AP9" s="6"/>
       <c r="AQ9" s="6"/>
     </row>
-    <row r="10" spans="1:43" ht="27" customHeight="1">
+    <row r="10" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>12</v>
       </c>
@@ -1272,7 +1291,7 @@
       <c r="AP10" s="6"/>
       <c r="AQ10" s="6"/>
     </row>
-    <row r="11" spans="1:43" ht="27" customHeight="1">
+    <row r="11" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1363,7 +1382,7 @@
       <c r="AP11" s="6"/>
       <c r="AQ11" s="6"/>
     </row>
-    <row r="12" spans="1:43" ht="27" customHeight="1">
+    <row r="12" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>10</v>
       </c>
@@ -1464,7 +1483,7 @@
       <c r="AP12" s="6"/>
       <c r="AQ12" s="6"/>
     </row>
-    <row r="13" spans="1:43" ht="27" customHeight="1">
+    <row r="13" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>9</v>
       </c>
@@ -1553,7 +1572,7 @@
       <c r="AP13" s="6"/>
       <c r="AQ13" s="6"/>
     </row>
-    <row r="14" spans="1:43" ht="27" customHeight="1">
+    <row r="14" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>8</v>
       </c>
@@ -1642,7 +1661,7 @@
       <c r="AP14" s="6"/>
       <c r="AQ14" s="6"/>
     </row>
-    <row r="15" spans="1:43" ht="27" customHeight="1">
+    <row r="15" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>7</v>
       </c>
@@ -1729,7 +1748,7 @@
       <c r="AP15" s="6"/>
       <c r="AQ15" s="6"/>
     </row>
-    <row r="16" spans="1:43" ht="27" customHeight="1">
+    <row r="16" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>6</v>
       </c>
@@ -1816,7 +1835,7 @@
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
     </row>
-    <row r="17" spans="3:43" ht="27" customHeight="1">
+    <row r="17" spans="3:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>5</v>
       </c>
@@ -1903,7 +1922,7 @@
       <c r="AP17" s="6"/>
       <c r="AQ17" s="6"/>
     </row>
-    <row r="18" spans="3:43" ht="27" customHeight="1">
+    <row r="18" spans="3:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>4</v>
       </c>
@@ -1990,7 +2009,7 @@
       <c r="AP18" s="6"/>
       <c r="AQ18" s="6"/>
     </row>
-    <row r="19" spans="3:43" ht="27" customHeight="1">
+    <row r="19" spans="3:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>3</v>
       </c>
@@ -2077,7 +2096,7 @@
       <c r="AP19" s="6"/>
       <c r="AQ19" s="6"/>
     </row>
-    <row r="20" spans="3:43" ht="27" customHeight="1">
+    <row r="20" spans="3:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>2</v>
       </c>
@@ -2164,7 +2183,7 @@
       <c r="AP20" s="6"/>
       <c r="AQ20" s="6"/>
     </row>
-    <row r="21" spans="3:43" ht="27" customHeight="1">
+    <row r="21" spans="3:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>1</v>
       </c>
@@ -2251,7 +2270,7 @@
       <c r="AP21" s="6"/>
       <c r="AQ21" s="6"/>
     </row>
-    <row r="22" spans="3:43" ht="27" customHeight="1">
+    <row r="22" spans="3:43" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D22" s="2">
         <v>0</v>
       </c>
@@ -2293,44 +2312,39 @@
       <c r="AP22" s="6"/>
       <c r="AQ22" s="6"/>
     </row>
-    <row r="23" spans="3:43">
+    <row r="23" spans="3:43" x14ac:dyDescent="0.2">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
         <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, true, false}, {true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, false, true, true, true, false, false, false, true, true}, {false, false, true, false, false, false, false, false, true, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
-    <row r="40" spans="7:7">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="C2:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="59" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
@@ -2338,12 +2352,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="3:5">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="10" t="s">
         <v>2</v>
       </c>
@@ -2354,7 +2368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
@@ -2365,7 +2379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
@@ -2378,934 +2392,692 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A3:E52"/>
+  <dimension ref="A2:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E52"/>
+      <selection activeCell="G3" sqref="G3:G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="7" max="7" width="80.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>CONCATENATE("go playGames(Strategy{Burn: ",A3,", Step:",E3,", BHoles:",B3,", FHoles:",C3,", HighY:",D3,"}, 22, false, false)")</f>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="E3" t="str">
-        <f>CONCATENATE("go playGames(",A3,",",B3,",",C3,",",D3,", 10, TRUE)")</f>
-        <v>go playGames(7,1,2,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G33" si="0">CONCATENATE("go playGames(Strategy{Burn: ",A4,", Step:",E4,", BHoles:",B4,", FHoles:",C4,", HighY:",D4,"}, 22, false, false)")</f>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:7, FHoles:4, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" ref="E4:E52" si="0">CONCATENATE("go playGames(",A4,",",B4,",",C4,",",D4,", 10, TRUE)")</f>
-        <v>go playGames(6,1,5,3, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,3,4,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:6, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,3,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(4,1,2,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:6, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:4, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>4</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,2,4,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,1,3,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:4, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:2, BHoles:6, FHoles:4, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:6, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
         <v>7</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,5,8, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,4,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:1, BHoles:4, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>6</v>
       </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,4,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:6, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:6, FHoles:4, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:7, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>3</v>
       </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13">
+      <c r="B17">
         <v>7</v>
       </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,3,6,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:4, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:3, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,2,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,2,3,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:5, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
         <v>7</v>
       </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,3,3, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
         <v>7</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17">
+      <c r="C21">
         <v>4</v>
       </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,6,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,5,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,2,4,3, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,2,2,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
       <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,5,3, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:4, FHoles:4, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:6, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:2, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:2, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>5</v>
       </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,2,5,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
+      <c r="B27">
         <v>7</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
         <v>5</v>
       </c>
-      <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,5,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:5, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:5, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
         <v>7</v>
       </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
         <v>3</v>
       </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,3,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>6</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 1, Step:2, BHoles:7, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
         <v>7</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,1,2,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,3,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
-        <v>6</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,2,4,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
-        <v>7</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,3,3,8, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>7</v>
-      </c>
-      <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,2,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>7</v>
-      </c>
-      <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,2,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>7</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,2,3,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <v>5</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32">
-        <v>6</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,2,3,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
         <v>3</v>
       </c>
-      <c r="D33">
-        <v>7</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,1,3,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <v>5</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
-      </c>
-      <c r="D34">
-        <v>4</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,5,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
-        <v>6</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
-      </c>
-      <c r="D35">
-        <v>8</v>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,1,5,8, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
-        <v>7</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36">
-        <v>7</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,4,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37">
-        <v>5</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>4</v>
-      </c>
-      <c r="E37" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,2,3,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38">
-        <v>5</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>5</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,2,3,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39">
-        <v>6</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,1,4,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40">
-        <v>7</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>8</v>
-      </c>
-      <c r="E40" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,6,8, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41">
-        <v>7</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-      <c r="D41">
-        <v>7</v>
-      </c>
-      <c r="E41" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,5,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-      <c r="D42">
-        <v>8</v>
-      </c>
-      <c r="E42" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,3,8, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43">
-        <v>7</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-      <c r="D43">
-        <v>7</v>
-      </c>
-      <c r="E43" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,3,7, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44">
-        <v>7</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
-      </c>
-      <c r="C44">
-        <v>4</v>
-      </c>
-      <c r="D44">
-        <v>8</v>
-      </c>
-      <c r="E44" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,2,4,8, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>4</v>
-      </c>
-      <c r="D45">
-        <v>5</v>
-      </c>
-      <c r="E45" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,4,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46">
-        <v>7</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
-        <v>5</v>
-      </c>
-      <c r="E46" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,1,2,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47">
-        <v>7</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47">
-        <v>3</v>
-      </c>
-      <c r="D47">
-        <v>6</v>
-      </c>
-      <c r="E47" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,3,3,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48">
-        <v>5</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="E48" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,2,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49">
-        <v>5</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>4</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-      <c r="E49" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,4,4, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50">
-        <v>5</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>3</v>
-      </c>
-      <c r="D50">
-        <v>5</v>
-      </c>
-      <c r="E50" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(5,1,3,5, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51">
-        <v>6</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>5</v>
-      </c>
-      <c r="D51">
-        <v>6</v>
-      </c>
-      <c r="E51" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(6,1,5,6, 10, TRUE)</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52">
-        <v>7</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>5</v>
-      </c>
-      <c r="E52" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(7,3,2,5, 10, TRUE)</v>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:7, FHoles:2, HighY:3}, 22, false, false)</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v 73 enforce  T-spin
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23960" yWindow="7880" windowWidth="19760" windowHeight="18820" tabRatio="500"/>
+    <workbookView xWindow="13740" yWindow="6480" windowWidth="19760" windowHeight="18820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="15">
   <si>
     <t>.</t>
   </si>
@@ -532,7 +532,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
@@ -1297,17 +1297,13 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="O11" t="str">
         <f t="shared" si="0"/>
@@ -1319,7 +1315,7 @@
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" si="9"/>
@@ -1343,7 +1339,7 @@
       </c>
       <c r="W11" t="str">
         <f t="shared" si="7"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="8"/>
@@ -1351,7 +1347,7 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, true, false, false, false, false, false, true, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF11" s="7" t="s">
         <v>0</v>
@@ -1386,31 +1382,19 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="1"/>
@@ -1418,15 +1402,15 @@
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="9"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="12"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="13"/>
@@ -1442,15 +1426,15 @@
       </c>
       <c r="W12" t="str">
         <f t="shared" si="7"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="8"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="4"/>
-        <v>{true, false, true, true, true, false, false, false, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>0</v>
@@ -1487,43 +1471,27 @@
       <c r="C13">
         <v>9</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="M13" s="1"/>
       <c r="O13" t="str">
         <f t="shared" ref="O13:O21" si="14">IF(D13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" ref="P13:P21" si="15">IF(E13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" ref="Q13:Q21" si="16">IF(F13=".","true","false")</f>
@@ -1531,23 +1499,23 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" ref="R13:R21" si="17">IF(G13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" ref="S13:S21" si="18">IF(H13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" ref="T13:T21" si="19">IF(I13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" ref="U13:U21" si="20">IF(J13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" ref="V13:V21" si="21">IF(K13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" ref="W13:W21" si="22">IF(L13=".","true","false")</f>
@@ -1555,11 +1523,11 @@
       </c>
       <c r="X13" t="str">
         <f t="shared" ref="X13:X21" si="23">IF(M13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{false, false, true, false, false, false, false, false, true, false}</v>
       </c>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
@@ -1579,9 +1547,7 @@
       <c r="D14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="7" t="s">
         <v>0</v>
       </c>
@@ -1591,15 +1557,9 @@
       <c r="H14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="7" t="s">
         <v>0</v>
       </c>
@@ -1612,7 +1572,7 @@
       </c>
       <c r="P14" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="16"/>
@@ -1628,15 +1588,15 @@
       </c>
       <c r="T14" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U14" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="22"/>
@@ -1648,7 +1608,7 @@
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, true, true, true, true, true}</v>
+        <v>{true, false, true, true, true, false, false, false, true, true}</v>
       </c>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
@@ -2280,9 +2240,7 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="G22" s="2">
-        <v>3</v>
-      </c>
+      <c r="G22" s="1"/>
       <c r="H22" s="2">
         <v>4</v>
       </c>
@@ -2315,7 +2273,7 @@
     <row r="23" spans="3:43" x14ac:dyDescent="0.2">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, true, false}, {true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, true, true, true, true}, {true, false, true, true, true, false, false, false, true, true}, {false, false, true, false, false, false, false, false, true, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, true, false}, {true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, false, true, true, true, false, false, false, true, true}, {false, false, true, false, false, false, false, false, true, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new analytics and strategy
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="6480" windowWidth="19760" windowHeight="18820" tabRatio="500"/>
+    <workbookView xWindow="9240" yWindow="5340" windowWidth="28460" windowHeight="20400" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
@@ -2356,10 +2356,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:G33"/>
+  <dimension ref="A2:G157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G33"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="G157" sqref="G3:G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2402,60 +2402,60 @@
       </c>
       <c r="G3" t="str">
         <f>CONCATENATE("go playGames(Strategy{Burn: ",A3,", Step:",E3,", BHoles:",B3,", FHoles:",C3,", HighY:",D3,"}, 22, false, false)")</f>
-        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:7, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G33" si="0">CONCATENATE("go playGames(Strategy{Burn: ",A4,", Step:",E4,", BHoles:",B4,", FHoles:",C4,", HighY:",D4,"}, 22, false, false)")</f>
-        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:7, FHoles:4, HighY:1}, 22, false, false)</v>
+        <f t="shared" ref="G4:G69" si="0">CONCATENATE("go playGames(Strategy{Burn: ",A4,", Step:",E4,", BHoles:",B4,", FHoles:",C4,", HighY:",D4,"}, 22, false, false)")</f>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:8, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:6, FHoles:4, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:6, FHoles:6, HighY:1}, 22, false, false)</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2465,49 +2465,49 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:3, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:6, FHoles:4, HighY:3}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:10, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:4, FHoles:3, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:5, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2515,41 +2515,41 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:4, FHoles:3, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:6, FHoles:4, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:2, BHoles:6, FHoles:4, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:6, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2557,31 +2557,31 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:6, FHoles:3, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:8, FHoles:6, HighY:4}, 22, false, false)</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -2591,49 +2591,49 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:4, HighY:3}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:8, FHoles:6, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 5, Step:1, BHoles:4, FHoles:2, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:8, FHoles:4, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:6, FHoles:4, HighY:3}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:10, FHoles:4, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2641,20 +2641,20 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:6, FHoles:4, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2665,217 +2665,217 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:7, FHoles:2, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:7, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:4, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:9, FHoles:5, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:3, HighY:4}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:9, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:1, BHoles:5, FHoles:2, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:8, FHoles:5, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:8, FHoles:1, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:8, FHoles:6, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:4, FHoles:4, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:10, FHoles:4, HighY:4}, 22, false, false)</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:6, FHoles:3, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:10, FHoles:5, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <v>7</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:2, HighY:4}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:3, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:2, HighY:4}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:10, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:8, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27">
         <v>7</v>
@@ -2899,140 +2899,2744 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:3, HighY:1}, 22, false, false)</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:2, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:6, FHoles:2, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:5, FHoles:4, HighY:2}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:10, FHoles:1, HighY:3}, 22, false, false)</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:5, FHoles:2, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:4, HighY:1}, 22, false, false)</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 1, Step:2, BHoles:7, FHoles:4, HighY:3}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:10, FHoles:3, HighY:1}, 22, false, false)</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:3, HighY:1}, 22, false, false)</v>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:10, FHoles:6, HighY:2}, 22, false, false)</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:9, FHoles:2, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:9, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:1, BHoles:10, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:6, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:6, FHoles:4, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:10, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:10, FHoles:3, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:10, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:9, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:9, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
         <v>7</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="0"/>
-        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:7, FHoles:2, HighY:3}, 22, false, false)</v>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:9, FHoles:3, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:5, FHoles:5, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:7, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:1, BHoles:8, FHoles:6, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:10, FHoles:5, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:6, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:8, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:9, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:6, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:10, FHoles:1, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:5, FHoles:6, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:8, FHoles:5, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:9, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:10, FHoles:1, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:10, FHoles:6, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:6, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:6, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:6, FHoles:5, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:6, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:8, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:8, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:8, FHoles:1, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" ref="G68" si="1">CONCATENATE("go playGames(Strategy{Burn: ",A68,", Step:",E68,", BHoles:",B68,", FHoles:",C68,", HighY:",D68,"}, 22, false, false)")</f>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:9, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>10</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="0"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:10, FHoles:5, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" ref="G70:G133" si="2">CONCATENATE("go playGames(Strategy{Burn: ",A70,", Step:",E70,", BHoles:",B70,", FHoles:",C70,", HighY:",D70,"}, 22, false, false)")</f>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:10, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>4</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>4</v>
+      </c>
+      <c r="B73">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>4</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:10, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="C75">
+        <v>6</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:10, FHoles:6, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>6</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:6, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <v>5</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:8, FHoles:5, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:4, BHoles:9, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:10, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:10, FHoles:2, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81">
+        <v>6</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:6, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:8, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>6</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:8, FHoles:6, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:9, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="B85">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:4, BHoles:10, FHoles:3, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>6</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:6, FHoles:3, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>7</v>
+      </c>
+      <c r="C87">
+        <v>6</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:9, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:10, FHoles:3, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>4</v>
+      </c>
+      <c r="B90">
+        <v>7</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>3</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:7, FHoles:1, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>4</v>
+      </c>
+      <c r="B91">
+        <v>7</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:7, FHoles:5, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="C92">
+        <v>6</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:7, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+      <c r="C93">
+        <v>6</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:9, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:8, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:9, FHoles:3, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>9</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:9, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>9</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97">
+        <v>3</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:9, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:6, FHoles:1, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99">
+        <v>7</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100">
+        <v>9</v>
+      </c>
+      <c r="C100">
+        <v>6</v>
+      </c>
+      <c r="D100">
+        <v>4</v>
+      </c>
+      <c r="E100">
+        <v>2</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:9, FHoles:6, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:4, BHoles:10, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>10</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <v>3</v>
+      </c>
+      <c r="E102">
+        <v>3</v>
+      </c>
+      <c r="G102" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:10, FHoles:2, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>6</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:6, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>3</v>
+      </c>
+      <c r="B104">
+        <v>7</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:7, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>3</v>
+      </c>
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>3</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="G105" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:10, FHoles:2, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <v>3</v>
+      </c>
+      <c r="G106" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:8, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>4</v>
+      </c>
+      <c r="B107">
+        <v>8</v>
+      </c>
+      <c r="C107">
+        <v>4</v>
+      </c>
+      <c r="D107">
+        <v>3</v>
+      </c>
+      <c r="E107">
+        <v>2</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:8, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>4</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+      <c r="C108">
+        <v>5</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:9, FHoles:5, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>4</v>
+      </c>
+      <c r="B109">
+        <v>9</v>
+      </c>
+      <c r="C109">
+        <v>6</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+      <c r="E109">
+        <v>3</v>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:9, FHoles:6, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>5</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+      <c r="C110">
+        <v>3</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+      <c r="E110">
+        <v>2</v>
+      </c>
+      <c r="G110" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:9, FHoles:3, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>5</v>
+      </c>
+      <c r="B111">
+        <v>9</v>
+      </c>
+      <c r="C111">
+        <v>5</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111">
+        <v>4</v>
+      </c>
+      <c r="G111" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:4, BHoles:9, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>5</v>
+      </c>
+      <c r="B112">
+        <v>9</v>
+      </c>
+      <c r="C112">
+        <v>6</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>3</v>
+      </c>
+      <c r="G112" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:9, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>2</v>
+      </c>
+      <c r="B113">
+        <v>6</v>
+      </c>
+      <c r="C113">
+        <v>6</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>3</v>
+      </c>
+      <c r="G113" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:6, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>7</v>
+      </c>
+      <c r="C114">
+        <v>5</v>
+      </c>
+      <c r="D114">
+        <v>2</v>
+      </c>
+      <c r="E114">
+        <v>3</v>
+      </c>
+      <c r="G114" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:3, BHoles:7, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>2</v>
+      </c>
+      <c r="B115">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115">
+        <v>2</v>
+      </c>
+      <c r="G115" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:9, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116">
+        <v>9</v>
+      </c>
+      <c r="C116">
+        <v>3</v>
+      </c>
+      <c r="D116">
+        <v>3</v>
+      </c>
+      <c r="E116">
+        <v>2</v>
+      </c>
+      <c r="G116" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:9, FHoles:3, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>2</v>
+      </c>
+      <c r="B117">
+        <v>10</v>
+      </c>
+      <c r="C117">
+        <v>4</v>
+      </c>
+      <c r="D117">
+        <v>4</v>
+      </c>
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="G117" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:10, FHoles:4, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="G118" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:1, BHoles:8, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>3</v>
+      </c>
+      <c r="B119">
+        <v>8</v>
+      </c>
+      <c r="C119">
+        <v>3</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <v>2</v>
+      </c>
+      <c r="G119" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:8, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>8</v>
+      </c>
+      <c r="C120">
+        <v>6</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+      <c r="E120">
+        <v>2</v>
+      </c>
+      <c r="G120" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:8, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>9</v>
+      </c>
+      <c r="C121">
+        <v>6</v>
+      </c>
+      <c r="D121">
+        <v>4</v>
+      </c>
+      <c r="E121">
+        <v>3</v>
+      </c>
+      <c r="G121" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:9, FHoles:6, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>4</v>
+      </c>
+      <c r="B122">
+        <v>6</v>
+      </c>
+      <c r="C122">
+        <v>6</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="G122" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:6, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>4</v>
+      </c>
+      <c r="B123">
+        <v>7</v>
+      </c>
+      <c r="C123">
+        <v>6</v>
+      </c>
+      <c r="D123">
+        <v>3</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="G123" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:7, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>4</v>
+      </c>
+      <c r="B124">
+        <v>8</v>
+      </c>
+      <c r="C124">
+        <v>5</v>
+      </c>
+      <c r="D124">
+        <v>4</v>
+      </c>
+      <c r="E124">
+        <v>2</v>
+      </c>
+      <c r="G124" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:8, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>4</v>
+      </c>
+      <c r="B125">
+        <v>8</v>
+      </c>
+      <c r="C125">
+        <v>6</v>
+      </c>
+      <c r="D125">
+        <v>4</v>
+      </c>
+      <c r="E125">
+        <v>2</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:8, FHoles:6, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>4</v>
+      </c>
+      <c r="B126">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>2</v>
+      </c>
+      <c r="G126" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:9, FHoles:1, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>4</v>
+      </c>
+      <c r="B127">
+        <v>10</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>2</v>
+      </c>
+      <c r="E127">
+        <v>4</v>
+      </c>
+      <c r="G127" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:4, BHoles:10, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>4</v>
+      </c>
+      <c r="B128">
+        <v>10</v>
+      </c>
+      <c r="C128">
+        <v>6</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>4</v>
+      </c>
+      <c r="G128" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:4, BHoles:10, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>4</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>6</v>
+      </c>
+      <c r="D129">
+        <v>3</v>
+      </c>
+      <c r="E129">
+        <v>2</v>
+      </c>
+      <c r="G129" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:10, FHoles:6, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>5</v>
+      </c>
+      <c r="B130">
+        <v>7</v>
+      </c>
+      <c r="C130">
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>3</v>
+      </c>
+      <c r="G130" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>5</v>
+      </c>
+      <c r="B131">
+        <v>9</v>
+      </c>
+      <c r="C131">
+        <v>5</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="G131" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:1, BHoles:9, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>5</v>
+      </c>
+      <c r="B132">
+        <v>10</v>
+      </c>
+      <c r="C132">
+        <v>3</v>
+      </c>
+      <c r="D132">
+        <v>4</v>
+      </c>
+      <c r="E132">
+        <v>3</v>
+      </c>
+      <c r="G132" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:10, FHoles:3, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>5</v>
+      </c>
+      <c r="B133">
+        <v>10</v>
+      </c>
+      <c r="C133">
+        <v>4</v>
+      </c>
+      <c r="D133">
+        <v>3</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="G133" t="str">
+        <f t="shared" si="2"/>
+        <v>go playGames(Strategy{Burn: 5, Step:1, BHoles:10, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>5</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+      <c r="C134">
+        <v>6</v>
+      </c>
+      <c r="D134">
+        <v>4</v>
+      </c>
+      <c r="E134">
+        <v>2</v>
+      </c>
+      <c r="G134" t="str">
+        <f t="shared" ref="G134:G157" si="3">CONCATENATE("go playGames(Strategy{Burn: ",A134,", Step:",E134,", BHoles:",B134,", FHoles:",C134,", HighY:",D134,"}, 22, false, false)")</f>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:10, FHoles:6, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>2</v>
+      </c>
+      <c r="B135">
+        <v>5</v>
+      </c>
+      <c r="C135">
+        <v>6</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+      <c r="G135" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:5, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136">
+        <v>8</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>3</v>
+      </c>
+      <c r="E136">
+        <v>2</v>
+      </c>
+      <c r="G136" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:8, FHoles:2, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137">
+        <v>9</v>
+      </c>
+      <c r="C137">
+        <v>6</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="G137" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 2, Step:1, BHoles:9, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>2</v>
+      </c>
+      <c r="B138">
+        <v>10</v>
+      </c>
+      <c r="C138">
+        <v>5</v>
+      </c>
+      <c r="D138">
+        <v>2</v>
+      </c>
+      <c r="E138">
+        <v>2</v>
+      </c>
+      <c r="G138" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 2, Step:2, BHoles:10, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>3</v>
+      </c>
+      <c r="B139">
+        <v>7</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>2</v>
+      </c>
+      <c r="E139">
+        <v>2</v>
+      </c>
+      <c r="G139" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:1, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>3</v>
+      </c>
+      <c r="B140">
+        <v>7</v>
+      </c>
+      <c r="C140">
+        <v>4</v>
+      </c>
+      <c r="D140">
+        <v>2</v>
+      </c>
+      <c r="E140">
+        <v>2</v>
+      </c>
+      <c r="G140" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:4, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="B141">
+        <v>7</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>2</v>
+      </c>
+      <c r="G141" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:7, FHoles:5, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>3</v>
+      </c>
+      <c r="B142">
+        <v>10</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+      <c r="D142">
+        <v>4</v>
+      </c>
+      <c r="E142">
+        <v>3</v>
+      </c>
+      <c r="G142" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 3, Step:3, BHoles:10, FHoles:3, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>3</v>
+      </c>
+      <c r="B143">
+        <v>10</v>
+      </c>
+      <c r="C143">
+        <v>4</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+      <c r="G143" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 3, Step:2, BHoles:10, FHoles:4, HighY:3}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>4</v>
+      </c>
+      <c r="B144">
+        <v>5</v>
+      </c>
+      <c r="C144">
+        <v>6</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>2</v>
+      </c>
+      <c r="G144" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:5, FHoles:6, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>4</v>
+      </c>
+      <c r="B145">
+        <v>6</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>2</v>
+      </c>
+      <c r="E145">
+        <v>3</v>
+      </c>
+      <c r="G145" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:6, FHoles:2, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>4</v>
+      </c>
+      <c r="B146">
+        <v>6</v>
+      </c>
+      <c r="C146">
+        <v>3</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>3</v>
+      </c>
+      <c r="G146" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:6, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>4</v>
+      </c>
+      <c r="B147">
+        <v>6</v>
+      </c>
+      <c r="C147">
+        <v>5</v>
+      </c>
+      <c r="D147">
+        <v>2</v>
+      </c>
+      <c r="E147">
+        <v>2</v>
+      </c>
+      <c r="G147" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:6, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>4</v>
+      </c>
+      <c r="B148">
+        <v>7</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>2</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="G148" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:7, FHoles:1, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>4</v>
+      </c>
+      <c r="B149">
+        <v>8</v>
+      </c>
+      <c r="C149">
+        <v>5</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>2</v>
+      </c>
+      <c r="G149" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:8, FHoles:5, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>4</v>
+      </c>
+      <c r="B150">
+        <v>8</v>
+      </c>
+      <c r="C150">
+        <v>6</v>
+      </c>
+      <c r="D150">
+        <v>2</v>
+      </c>
+      <c r="E150">
+        <v>3</v>
+      </c>
+      <c r="G150" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:3, BHoles:8, FHoles:6, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>4</v>
+      </c>
+      <c r="B151">
+        <v>9</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
+      </c>
+      <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="G151" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:1, BHoles:9, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>4</v>
+      </c>
+      <c r="B152">
+        <v>10</v>
+      </c>
+      <c r="C152">
+        <v>3</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>2</v>
+      </c>
+      <c r="G152" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 4, Step:2, BHoles:10, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>5</v>
+      </c>
+      <c r="B153">
+        <v>8</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>3</v>
+      </c>
+      <c r="G153" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:8, FHoles:2, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>5</v>
+      </c>
+      <c r="B154">
+        <v>8</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+      <c r="E154">
+        <v>3</v>
+      </c>
+      <c r="G154" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 5, Step:3, BHoles:8, FHoles:3, HighY:1}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>5</v>
+      </c>
+      <c r="B155">
+        <v>8</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
+      </c>
+      <c r="D155">
+        <v>4</v>
+      </c>
+      <c r="E155">
+        <v>2</v>
+      </c>
+      <c r="G155" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:8, FHoles:5, HighY:4}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>5</v>
+      </c>
+      <c r="B156">
+        <v>9</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156">
+        <v>2</v>
+      </c>
+      <c r="E156">
+        <v>2</v>
+      </c>
+      <c r="G156" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:9, FHoles:5, HighY:2}, 22, false, false)</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>5</v>
+      </c>
+      <c r="B157">
+        <v>10</v>
+      </c>
+      <c r="C157">
+        <v>3</v>
+      </c>
+      <c r="D157">
+        <v>4</v>
+      </c>
+      <c r="E157">
+        <v>2</v>
+      </c>
+      <c r="G157" t="str">
+        <f t="shared" si="3"/>
+        <v>go playGames(Strategy{Burn: 5, Step:2, BHoles:10, FHoles:3, HighY:4}, 22, false, false)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Step calculation is fixed
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="5340" windowWidth="28460" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="18180" yWindow="6540" windowWidth="15220" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="15">
   <si>
     <t>.</t>
   </si>
@@ -1298,15 +1298,9 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1325,15 +1319,15 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" si="9"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="12"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="13"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" si="10"/>
@@ -1353,7 +1347,7 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, true, true, true, false, false, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF11" s="7" t="s">
         <v>0</v>
@@ -1391,9 +1385,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1414,7 +1406,7 @@
       </c>
       <c r="R12" t="str">
         <f t="shared" si="9"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="12"/>
@@ -1442,7 +1434,7 @@
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, true, false, false, false, false, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>0</v>
@@ -1481,21 +1473,13 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="O13" t="str">
         <f t="shared" ref="O13:O21" si="14">IF(D13=".","true","false")</f>
@@ -1507,15 +1491,15 @@
       </c>
       <c r="Q13" t="str">
         <f t="shared" ref="Q13:Q21" si="16">IF(F13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ref="R13:R21" si="17">IF(G13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" ref="S13:S21" si="18">IF(H13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" ref="T13:T21" si="19">IF(I13=".","true","false")</f>
@@ -1531,7 +1515,7 @@
       </c>
       <c r="W13" t="str">
         <f t="shared" ref="W13:W21" si="22">IF(L13=".","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" ref="X13:X21" si="23">IF(M13=".","true","false")</f>
@@ -1539,7 +1523,7 @@
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, true, true, true, false, false, false, true, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
@@ -1556,49 +1540,35 @@
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="O14" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" si="19"/>
@@ -1614,15 +1584,15 @@
       </c>
       <c r="W14" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X14" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, false, false, false, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
@@ -1639,57 +1609,39 @@
       <c r="C15">
         <v>7</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="O15" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="20"/>
@@ -1697,19 +1649,19 @@
       </c>
       <c r="V15" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, true, false, true, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -1726,37 +1678,19 @@
       <c r="C16">
         <v>6</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
       <c r="O16" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="15"/>
@@ -1764,39 +1698,39 @@
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="4"/>
-        <v>{true, false, true, true, true, true, true, true, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -1813,69 +1747,51 @@
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="O17" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="23"/>
@@ -1883,7 +1799,7 @@
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, true, true, true, true, false}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -1900,61 +1816,43 @@
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
       <c r="O18" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T18" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U18" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="21"/>
@@ -1962,15 +1860,15 @@
       </c>
       <c r="W18" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X18" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, true, true, false, true, true}</v>
+        <v>{false, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -1987,41 +1885,25 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="M19" s="1"/>
       <c r="O19" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="16"/>
@@ -2029,23 +1911,23 @@
       </c>
       <c r="R19" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T19" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U19" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="22"/>
@@ -2053,11 +1935,11 @@
       </c>
       <c r="X19" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, true, true, true, true, false, true}</v>
+        <v>{false, false, true, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -2074,41 +1956,25 @@
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
       <c r="O20" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="16"/>
@@ -2116,7 +1982,7 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="18"/>
@@ -2124,27 +1990,27 @@
       </c>
       <c r="T20" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U20" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W20" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X20" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, true, false, true, true, true, true, true}</v>
+        <v>{false, false, true, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -2161,41 +2027,27 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
       <c r="O21" t="str">
         <f t="shared" si="14"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="15"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="16"/>
@@ -2203,35 +2055,35 @@
       </c>
       <c r="R21" t="str">
         <f t="shared" si="17"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" si="19"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="20"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="21"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="W21" t="str">
         <f t="shared" si="22"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" si="23"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="4"/>
-        <v>{true, true, true, false, true, true, true, true, true, true}</v>
+        <v>{false, false, true, true, false, false, false, false, false, false}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -2289,7 +2141,7 @@
     <row r="23" spans="3:43" x14ac:dyDescent="0.2">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{true, true, true, false, true, true, true, true, true, true}, {true, true, true, true, false, true, true, true, true, true}, {true, true, true, true, true, true, true, true, false, true}, {true, true, true, true, true, true, true, false, true, true}, {true, true, true, true, true, true, true, true, true, false}, {true, false, true, true, true, true, true, true, true, true}, {true, true, true, true, true, true, false, true, true, true}, {true, true, true, true, true, false, false, false, true, true}, {false, false, true, true, true, false, false, false, true, false}, {false, false, false, true, false, false, false, false, false, false}, {false, false, false, true, true, true, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{false, false, true, true, false, false, false, false, false, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
sets created for bug when fixing holes
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18180" yWindow="6540" windowWidth="15220" windowHeight="19440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="15">
   <si>
     <t>.</t>
   </si>
@@ -533,7 +533,7 @@
   <dimension ref="A1:AQ40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1887,16 +1887,18 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="L19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O19" t="str">
         <f t="shared" si="14"/>
         <v>false</v>
@@ -1907,7 +1909,7 @@
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" si="17"/>
@@ -1931,15 +1933,15 @@
       </c>
       <c r="W19" t="str">
         <f t="shared" si="22"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="23"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, true, false, false, false, false, false, false, false}</v>
+        <v>{false, false, false, false, false, false, false, false, true, true}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -1961,13 +1963,27 @@
       <c r="F20" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="G20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O20" t="str">
         <f t="shared" si="14"/>
         <v>false</v>
@@ -1982,35 +1998,35 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="17"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="18"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T20" t="str">
         <f t="shared" si="19"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U20" t="str">
         <f t="shared" si="20"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="21"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W20" t="str">
         <f t="shared" si="22"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X20" t="str">
         <f t="shared" si="23"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, true, false, false, false, false, false, false, false}</v>
+        <v>{false, false, true, true, true, true, true, true, true, true}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -2029,18 +2045,26 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O21" t="str">
         <f t="shared" si="14"/>
         <v>false</v>
@@ -2051,39 +2075,39 @@
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="16"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="R21" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="18"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" si="19"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="20"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="21"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="W21" t="str">
         <f t="shared" si="22"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" si="23"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, true, true, false, false, false, false, false, false}</v>
+        <v>{false, false, false, false, true, true, true, true, true, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -2141,7 +2165,7 @@
     <row r="23" spans="3:43" x14ac:dyDescent="0.2">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{false, false, true, true, false, false, false, false, false, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, true, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{false, false, false, false, true, true, true, true, true, true}, {false, false, true, true, true, true, true, true, true, true}, {false, false, false, false, false, false, false, false, true, true}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding game test for detected bug. And fix for Tspin detection bug
</commit_message>
<xml_diff>
--- a/analitics/tetris.xlsx
+++ b/analitics/tetris.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="-10340" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="59000" yWindow="-7440" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="visual" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="15">
   <si>
     <t>.</t>
   </si>
@@ -1747,7 +1747,9 @@
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1759,7 +1761,7 @@
       <c r="M17" s="1"/>
       <c r="O17" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="15"/>
@@ -1799,7 +1801,7 @@
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{true, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -1816,7 +1818,9 @@
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1828,7 +1832,7 @@
       <c r="M18" s="1"/>
       <c r="O18" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="15"/>
@@ -1868,7 +1872,7 @@
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{true, false, false, false, false, false, false, false, false, false}</v>
       </c>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -1885,27 +1889,35 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="M19" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O19" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" si="17"/>
@@ -1933,11 +1945,11 @@
       </c>
       <c r="X19" t="str">
         <f t="shared" si="23"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, false, false, false, false, false, false, false}</v>
+        <v>{true, true, true, false, false, false, false, false, false, true}</v>
       </c>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -1954,39 +1966,43 @@
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="M20" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O20" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="17"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="18"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="T20" t="str">
         <f t="shared" si="19"/>
@@ -2006,11 +2022,11 @@
       </c>
       <c r="X20" t="str">
         <f t="shared" si="23"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, true, true, false, false, false, false, false}</v>
+        <v>{true, true, true, false, false, false, false, false, false, true}</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -2027,9 +2043,15 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="7" t="s">
         <v>0</v>
@@ -2040,18 +2062,20 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="M21" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="O21" t="str">
         <f t="shared" si="14"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="15"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="16"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="R21" t="str">
         <f t="shared" si="17"/>
@@ -2079,11 +2103,11 @@
       </c>
       <c r="X21" t="str">
         <f t="shared" si="23"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="4"/>
-        <v>{false, false, false, false, true, true, false, false, false, false}</v>
+        <v>{true, true, true, false, true, true, false, false, false, true}</v>
       </c>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -2141,7 +2165,7 @@
     <row r="23" spans="3:43" x14ac:dyDescent="0.2">
       <c r="Z23" t="str">
         <f>CONCATENATE("{",Z21,", ",Z20,", ",Z19,", ",Z18,", ",Z17,", ",Z16,", ",Z15,", ",Z14,", ",Z13,", ",Z12,", ",Z11,", ",Z10,", ",Z9,", ",Z8,", ",Z7,", ",Z6,", ",Z5,", ",Z4,", ",Z3,", ",Z2,"}")</f>
-        <v>{{false, false, false, false, true, true, false, false, false, false}, {false, false, false, true, true, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
+        <v>{{true, true, true, false, true, true, false, false, false, true}, {true, true, true, false, false, false, false, false, false, true}, {true, true, true, false, false, false, false, false, false, true}, {true, false, false, false, false, false, false, false, false, false}, {true, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}, {false, false, false, false, false, false, false, false, false, false}}</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>